<commit_message>
Update PBO and SC for 12/31/22 LDI Dash board
</commit_message>
<xml_diff>
--- a/data/time_series/past_pbo_cashflow_data.xlsx
+++ b/data/time_series/past_pbo_cashflow_data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\UPS_MV\data\time_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD668AB-8655-473B-B07C-7018587D7BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22088D03-DE4A-4C34-8957-A7F8CEF73D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="26370" windowHeight="15435" activeTab="3" xr2:uid="{D884DE58-9E6E-4B5F-AB9A-D4EA4714C804}"/>
+    <workbookView xWindow="-57710" yWindow="-110" windowWidth="29020" windowHeight="15820" activeTab="4" xr2:uid="{D884DE58-9E6E-4B5F-AB9A-D4EA4714C804}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
     <sheet name="2020" sheetId="2" r:id="rId2"/>
     <sheet name="2021" sheetId="3" r:id="rId3"/>
     <sheet name="2021_1" sheetId="4" r:id="rId4"/>
+    <sheet name="2022" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
@@ -55,13 +56,35 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,14 +104,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{2C03BA70-C8C3-411B-8BA7-437DCCEB6D37}"/>
+    <cellStyle name="Comma 2 2" xfId="3" xr:uid="{5D30E948-02B1-4D33-A7EB-24DED7B761FD}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,18 +432,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451252B7-47B5-4190-93D8-F75CC245F825}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43465</v>
       </c>
@@ -439,8 +473,9 @@
       <c r="D2">
         <v>344294440</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>EOMONTH(A2,12)</f>
         <v>43830</v>
@@ -455,7 +490,7 @@
         <v>396991026</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">EOMONTH(A3,12)</f>
         <v>44196</v>
@@ -470,7 +505,7 @@
         <v>435561482</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>44561</v>
@@ -485,7 +520,7 @@
         <v>471160143</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>44926</v>
@@ -500,7 +535,7 @@
         <v>502970192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>45291</v>
@@ -515,7 +550,7 @@
         <v>530763479</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>45657</v>
@@ -530,7 +565,7 @@
         <v>554923718</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>46022</v>
@@ -545,7 +580,7 @@
         <v>575182657</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>46387</v>
@@ -560,7 +595,7 @@
         <v>593468682</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>46752</v>
@@ -575,7 +610,7 @@
         <v>608975504</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>47118</v>
@@ -590,7 +625,7 @@
         <v>621155735</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>47483</v>
@@ -605,7 +640,7 @@
         <v>630301958</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>47848</v>
@@ -620,7 +655,7 @@
         <v>636784633</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>48213</v>
@@ -635,7 +670,7 @@
         <v>641677323</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>48579</v>
@@ -650,7 +685,7 @@
         <v>644821286</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>48944</v>
@@ -665,7 +700,7 @@
         <v>646001587</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>49309</v>
@@ -680,7 +715,7 @@
         <v>645038165</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>49674</v>
@@ -695,7 +730,7 @@
         <v>642357653</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>50040</v>
@@ -710,7 +745,7 @@
         <v>639182626</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>50405</v>
@@ -725,7 +760,7 @@
         <v>635628272</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>50770</v>
@@ -740,7 +775,7 @@
         <v>630828891</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>51135</v>
@@ -755,7 +790,7 @@
         <v>624321410</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>51501</v>
@@ -770,7 +805,7 @@
         <v>616016335</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>51866</v>
@@ -785,7 +820,7 @@
         <v>605956400</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>52231</v>
@@ -800,7 +835,7 @@
         <v>594198620</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>52596</v>
@@ -815,7 +850,7 @@
         <v>580852600</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>52962</v>
@@ -830,7 +865,7 @@
         <v>565975114</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>53327</v>
@@ -845,7 +880,7 @@
         <v>549572306</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>53692</v>
@@ -860,7 +895,7 @@
         <v>531801358</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>54057</v>
@@ -875,7 +910,7 @@
         <v>512750323</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>54423</v>
@@ -890,7 +925,7 @@
         <v>492555544</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>54788</v>
@@ -905,7 +940,7 @@
         <v>471450416</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>55153</v>
@@ -920,7 +955,7 @@
         <v>449547783</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>55518</v>
@@ -935,7 +970,7 @@
         <v>426988977</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>55884</v>
@@ -950,7 +985,7 @@
         <v>403976209</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>56249</v>
@@ -965,7 +1000,7 @@
         <v>380720176</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>56614</v>
@@ -980,7 +1015,7 @@
         <v>357400367</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>56979</v>
@@ -995,7 +1030,7 @@
         <v>334218090</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>57345</v>
@@ -1010,7 +1045,7 @@
         <v>311373502</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>57710</v>
@@ -1025,7 +1060,7 @@
         <v>289016959</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>58075</v>
@@ -1040,7 +1075,7 @@
         <v>267276548</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>58440</v>
@@ -1055,7 +1090,7 @@
         <v>246265911</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>58806</v>
@@ -1070,7 +1105,7 @@
         <v>226085111</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>59171</v>
@@ -1085,7 +1120,7 @@
         <v>206812880</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>59536</v>
@@ -1100,7 +1135,7 @@
         <v>188506943</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>59901</v>
@@ -1115,7 +1150,7 @@
         <v>171211518</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>60267</v>
@@ -1130,7 +1165,7 @@
         <v>154951678</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>60632</v>
@@ -1145,7 +1180,7 @@
         <v>139735436</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>60997</v>
@@ -1160,7 +1195,7 @@
         <v>125557105</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>61362</v>
@@ -1175,7 +1210,7 @@
         <v>112401468</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>61728</v>
@@ -1190,7 +1225,7 @@
         <v>100244785</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>62093</v>
@@ -1205,7 +1240,7 @@
         <v>89054951</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>62458</v>
@@ -1220,7 +1255,7 @@
         <v>78794183</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>62823</v>
@@ -1235,7 +1270,7 @@
         <v>69421192</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>63189</v>
@@ -1250,7 +1285,7 @@
         <v>60892235</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>63554</v>
@@ -1265,7 +1300,7 @@
         <v>53162437</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>63919</v>
@@ -1280,7 +1315,7 @@
         <v>46186582</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>64284</v>
@@ -1295,7 +1330,7 @@
         <v>39919084</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>64650</v>
@@ -1310,7 +1345,7 @@
         <v>34314181</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>65015</v>
@@ -1325,7 +1360,7 @@
         <v>29326144</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>65380</v>
@@ -1340,7 +1375,7 @@
         <v>24909747</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>65745</v>
@@ -1355,7 +1390,7 @@
         <v>21020872</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>66111</v>
@@ -1370,7 +1405,7 @@
         <v>17616527</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>66476</v>
@@ -1385,7 +1420,7 @@
         <v>14655169</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>66841</v>
@@ -1400,7 +1435,7 @@
         <v>12097004</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>67206</v>
@@ -1415,7 +1450,7 @@
         <v>9903508</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <f t="shared" ref="A68:A81" si="1">EOMONTH(A67,12)</f>
         <v>67572</v>
@@ -1430,7 +1465,7 @@
         <v>8037689</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <f t="shared" si="1"/>
         <v>67937</v>
@@ -1445,7 +1480,7 @@
         <v>6464039</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <f t="shared" si="1"/>
         <v>68302</v>
@@ -1460,7 +1495,7 @@
         <v>5148739</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <f t="shared" si="1"/>
         <v>68667</v>
@@ -1475,7 +1510,7 @@
         <v>4059795</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <f t="shared" si="1"/>
         <v>69033</v>
@@ -1490,7 +1525,7 @@
         <v>3167156</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <f t="shared" si="1"/>
         <v>69398</v>
@@ -1505,7 +1540,7 @@
         <v>2443017</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <f t="shared" si="1"/>
         <v>69763</v>
@@ -1520,7 +1555,7 @@
         <v>1862002</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <f t="shared" si="1"/>
         <v>70128</v>
@@ -1535,7 +1570,7 @@
         <v>1401202</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <f t="shared" si="1"/>
         <v>70494</v>
@@ -1550,7 +1585,7 @@
         <v>1040277</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <f t="shared" si="1"/>
         <v>70859</v>
@@ -1565,7 +1600,7 @@
         <v>761370</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <f t="shared" si="1"/>
         <v>71224</v>
@@ -1580,7 +1615,7 @@
         <v>548952</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
         <v>71589</v>
@@ -1595,7 +1630,7 @@
         <v>389682</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
         <v>71955</v>
@@ -1610,7 +1645,7 @@
         <v>272241</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
         <v>72320</v>
@@ -1635,15 +1670,16 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43830</v>
       </c>
@@ -1671,7 +1707,7 @@
         <v>393947712</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44196</v>
       </c>
@@ -1685,7 +1721,7 @@
         <v>460738936</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44561</v>
       </c>
@@ -1699,7 +1735,7 @@
         <v>501900129</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44926</v>
       </c>
@@ -1713,7 +1749,7 @@
         <v>540702732</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45291</v>
       </c>
@@ -1727,7 +1763,7 @@
         <v>575651821</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45657</v>
       </c>
@@ -1741,7 +1777,7 @@
         <v>605878635</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>46022</v>
       </c>
@@ -1755,7 +1791,7 @@
         <v>632205744</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>46387</v>
       </c>
@@ -1769,7 +1805,7 @@
         <v>656449549</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>46752</v>
       </c>
@@ -1783,7 +1819,7 @@
         <v>677698042</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>47118</v>
       </c>
@@ -1797,7 +1833,7 @@
         <v>695234160</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>47483</v>
       </c>
@@ -1811,7 +1847,7 @@
         <v>709232431</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>47848</v>
       </c>
@@ -1825,7 +1861,7 @@
         <v>720238255</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>48213</v>
       </c>
@@ -1839,7 +1875,7 @@
         <v>729181644</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>48579</v>
       </c>
@@ -1853,7 +1889,7 @@
         <v>735822645</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>48944</v>
       </c>
@@ -1867,7 +1903,7 @@
         <v>740004690</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>49309</v>
       </c>
@@ -1881,7 +1917,7 @@
         <v>741537991</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>49674</v>
       </c>
@@ -1895,7 +1931,7 @@
         <v>740862572</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>50040</v>
       </c>
@@ -1909,7 +1945,7 @@
         <v>739165640</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>50405</v>
       </c>
@@ -1923,7 +1959,7 @@
         <v>736546765</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>50770</v>
       </c>
@@ -1937,7 +1973,7 @@
         <v>732184483</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>51135</v>
       </c>
@@ -1951,7 +1987,7 @@
         <v>725674966</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>51501</v>
       </c>
@@ -1965,7 +2001,7 @@
         <v>716973874</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>51866</v>
       </c>
@@ -1979,7 +2015,7 @@
         <v>706124250</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>52231</v>
       </c>
@@ -1993,7 +2029,7 @@
         <v>693207228</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>52596</v>
       </c>
@@ -2007,7 +2043,7 @@
         <v>678397181</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>52962</v>
       </c>
@@ -2021,7 +2057,7 @@
         <v>661746773</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>53327</v>
       </c>
@@ -2035,7 +2071,7 @@
         <v>643299581</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>53692</v>
       </c>
@@ -2049,7 +2085,7 @@
         <v>623243047</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>54057</v>
       </c>
@@ -2063,7 +2099,7 @@
         <v>601669616</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>54423</v>
       </c>
@@ -2077,7 +2113,7 @@
         <v>578751828</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>54788</v>
       </c>
@@ -2091,7 +2127,7 @@
         <v>554722528</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>55153</v>
       </c>
@@ -2105,7 +2141,7 @@
         <v>529711495</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>55518</v>
       </c>
@@ -2119,7 +2155,7 @@
         <v>503891677</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>55884</v>
       </c>
@@ -2133,7 +2169,7 @@
         <v>477485436</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>56249</v>
       </c>
@@ -2147,7 +2183,7 @@
         <v>450735261</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>56614</v>
       </c>
@@ -2161,7 +2197,7 @@
         <v>423836855</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>56979</v>
       </c>
@@ -2175,7 +2211,7 @@
         <v>396999701</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>57345</v>
       </c>
@@ -2189,7 +2225,7 @@
         <v>370486217</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>57710</v>
       </c>
@@ -2203,7 +2239,7 @@
         <v>344508033</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>58075</v>
       </c>
@@ -2217,7 +2253,7 @@
         <v>319217574</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>58440</v>
       </c>
@@ -2231,7 +2267,7 @@
         <v>294743813</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>58806</v>
       </c>
@@ -2245,7 +2281,7 @@
         <v>271207636</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>59171</v>
       </c>
@@ -2259,7 +2295,7 @@
         <v>248706855</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>59536</v>
       </c>
@@ -2273,7 +2309,7 @@
         <v>227313802</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>59901</v>
       </c>
@@ -2287,7 +2323,7 @@
         <v>207083845</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>60267</v>
       </c>
@@ -2301,7 +2337,7 @@
         <v>188047787</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>60632</v>
       </c>
@@ -2315,7 +2351,7 @@
         <v>170214658</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>60997</v>
       </c>
@@ -2329,7 +2365,7 @@
         <v>153574909</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>61362</v>
       </c>
@@ -2343,7 +2379,7 @@
         <v>138106432</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>61728</v>
       </c>
@@ -2357,7 +2393,7 @@
         <v>123780633</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>62093</v>
       </c>
@@ -2371,7 +2407,7 @@
         <v>110560386</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>62458</v>
       </c>
@@ -2385,7 +2421,7 @@
         <v>98400281</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>62823</v>
       </c>
@@ -2399,7 +2435,7 @@
         <v>87251208</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>63189</v>
       </c>
@@ -2413,7 +2449,7 @@
         <v>77062252</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>63554</v>
       </c>
@@ -2427,7 +2463,7 @@
         <v>67781845</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>63919</v>
       </c>
@@ -2441,7 +2477,7 @@
         <v>59358899</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>64284</v>
       </c>
@@ -2455,7 +2491,7 @@
         <v>51742945</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>64650</v>
       </c>
@@ -2469,7 +2505,7 @@
         <v>44884003</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>65015</v>
       </c>
@@ -2483,7 +2519,7 @@
         <v>38732519</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>65380</v>
       </c>
@@ -2497,7 +2533,7 @@
         <v>33239648</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>65745</v>
       </c>
@@ -2511,7 +2547,7 @@
         <v>28357923</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>66111</v>
       </c>
@@ -2525,7 +2561,7 @@
         <v>24041288</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>66476</v>
       </c>
@@ -2539,7 +2575,7 @@
         <v>20245304</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>66841</v>
       </c>
@@ -2553,7 +2589,7 @@
         <v>16927456</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>67206</v>
       </c>
@@ -2567,7 +2603,7 @@
         <v>14046547</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>67572</v>
       </c>
@@ -2581,7 +2617,7 @@
         <v>11562809</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67937</v>
       </c>
@@ -2595,7 +2631,7 @@
         <v>9437786</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68302</v>
       </c>
@@ -2609,7 +2645,7 @@
         <v>7634478</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68667</v>
       </c>
@@ -2623,7 +2659,7 @@
         <v>6117455</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69033</v>
       </c>
@@ -2637,7 +2673,7 @@
         <v>4852920</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>69398</v>
       </c>
@@ -2651,7 +2687,7 @@
         <v>3809036</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>69763</v>
       </c>
@@ -2665,7 +2701,7 @@
         <v>2956132</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>70128</v>
       </c>
@@ -2679,7 +2715,7 @@
         <v>2266789</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>70494</v>
       </c>
@@ -2693,7 +2729,7 @@
         <v>1716066</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>70859</v>
       </c>
@@ -2707,7 +2743,7 @@
         <v>1281567</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>71224</v>
       </c>
@@ -2721,7 +2757,7 @@
         <v>943407</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>71589</v>
       </c>
@@ -2735,7 +2771,7 @@
         <v>684073</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>71955</v>
       </c>
@@ -2749,7 +2785,7 @@
         <v>488295</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>72320</v>
       </c>
@@ -2763,7 +2799,7 @@
         <v>342957</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>72685</v>
       </c>
@@ -2787,16 +2823,17 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2810,11 +2847,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44196</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1126020461</v>
       </c>
       <c r="C2">
@@ -2824,7 +2861,7 @@
         <v>372907665</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44561</v>
       </c>
@@ -2838,7 +2875,7 @@
         <v>409584297</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -2852,7 +2889,7 @@
         <v>443363866</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45291</v>
       </c>
@@ -2866,7 +2903,7 @@
         <v>474322697</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45657</v>
       </c>
@@ -2880,7 +2917,7 @@
         <v>604035023</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>46022</v>
       </c>
@@ -2894,7 +2931,7 @@
         <v>740660016</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>46387</v>
       </c>
@@ -2908,7 +2945,7 @@
         <v>784221239</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>46752</v>
       </c>
@@ -2922,7 +2959,7 @@
         <v>824102268</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>47118</v>
       </c>
@@ -2936,7 +2973,7 @@
         <v>859664062</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>47483</v>
       </c>
@@ -2950,7 +2987,7 @@
         <v>891752980</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>47848</v>
       </c>
@@ -2964,7 +3001,7 @@
         <v>920013262</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>48213</v>
       </c>
@@ -2978,7 +3015,7 @@
         <v>943743374</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>48579</v>
       </c>
@@ -2992,7 +3029,7 @@
         <v>963534950</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>48944</v>
       </c>
@@ -3006,7 +3043,7 @@
         <v>979037199</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>49309</v>
       </c>
@@ -3020,7 +3057,7 @@
         <v>989862991</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>49674</v>
       </c>
@@ -3034,7 +3071,7 @@
         <v>996418420</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>50040</v>
       </c>
@@ -3048,7 +3085,7 @@
         <v>999454236</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>50405</v>
       </c>
@@ -3062,7 +3099,7 @@
         <v>999179408</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>50770</v>
       </c>
@@ -3076,7 +3113,7 @@
         <v>995536423</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>51135</v>
       </c>
@@ -3090,7 +3127,7 @@
         <v>988367253</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>51501</v>
       </c>
@@ -3104,7 +3141,7 @@
         <v>977666859</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>51866</v>
       </c>
@@ -3118,7 +3155,7 @@
         <v>963572596</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>52231</v>
       </c>
@@ -3132,7 +3169,7 @@
         <v>946266764</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>52596</v>
       </c>
@@ -3146,7 +3183,7 @@
         <v>926120664</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>52962</v>
       </c>
@@ -3160,7 +3197,7 @@
         <v>903281871</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>53327</v>
       </c>
@@ -3174,7 +3211,7 @@
         <v>877892822</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>53692</v>
       </c>
@@ -3188,7 +3225,7 @@
         <v>850226546</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>54057</v>
       </c>
@@ -3202,7 +3239,7 @@
         <v>820402452</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>54423</v>
       </c>
@@ -3216,7 +3253,7 @@
         <v>788725581</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>54788</v>
       </c>
@@ -3230,7 +3267,7 @@
         <v>755505824</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>55153</v>
       </c>
@@ -3244,7 +3281,7 @@
         <v>720941992</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>55518</v>
       </c>
@@ -3258,7 +3295,7 @@
         <v>685318015</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>55884</v>
       </c>
@@ -3272,7 +3309,7 @@
         <v>648925327</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>56249</v>
       </c>
@@ -3286,7 +3323,7 @@
         <v>612090133</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>56614</v>
       </c>
@@ -3300,7 +3337,7 @@
         <v>575068927</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>56979</v>
       </c>
@@ -3314,7 +3351,7 @@
         <v>538141577</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>57345</v>
       </c>
@@ -3328,7 +3365,7 @@
         <v>501652998</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>57710</v>
       </c>
@@ -3342,7 +3379,7 @@
         <v>465907565</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>58075</v>
       </c>
@@ -3356,7 +3393,7 @@
         <v>431164743</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>58440</v>
       </c>
@@ -3370,7 +3407,7 @@
         <v>397612059</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>58806</v>
       </c>
@@ -3384,7 +3421,7 @@
         <v>365423548</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>59171</v>
       </c>
@@ -3398,7 +3435,7 @@
         <v>334744520</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>59536</v>
       </c>
@@ -3412,7 +3449,7 @@
         <v>305672506</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>59901</v>
       </c>
@@ -3426,7 +3463,7 @@
         <v>278285043</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>60267</v>
       </c>
@@ -3440,7 +3477,7 @@
         <v>252622894</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>60632</v>
       </c>
@@ -3454,7 +3491,7 @@
         <v>228688674</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>60997</v>
       </c>
@@ -3468,7 +3505,7 @@
         <v>206454576</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>61362</v>
       </c>
@@ -3482,7 +3519,7 @@
         <v>185874908</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>61728</v>
       </c>
@@ -3496,7 +3533,7 @@
         <v>166891591</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>62093</v>
       </c>
@@ -3510,7 +3547,7 @@
         <v>149435555</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>62458</v>
       </c>
@@ -3524,7 +3561,7 @@
         <v>133429789</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>62823</v>
       </c>
@@ -3538,7 +3575,7 @@
         <v>118790320</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>63189</v>
       </c>
@@ -3552,7 +3589,7 @@
         <v>105431095</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>63554</v>
       </c>
@@ -3566,7 +3603,7 @@
         <v>93267716</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>63919</v>
       </c>
@@ -3580,7 +3617,7 @@
         <v>82219151</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>64284</v>
       </c>
@@ -3594,7 +3631,7 @@
         <v>72208012</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>64650</v>
       </c>
@@ -3608,7 +3645,7 @@
         <v>63160909</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>65015</v>
       </c>
@@ -3622,7 +3659,7 @@
         <v>55008097</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>65380</v>
       </c>
@@ -3636,7 +3673,7 @@
         <v>47683537</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>65745</v>
       </c>
@@ -3650,7 +3687,7 @@
         <v>41125290</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>66111</v>
       </c>
@@ -3664,7 +3701,7 @@
         <v>35275092</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>66476</v>
       </c>
@@ -3678,7 +3715,7 @@
         <v>30078398</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>66841</v>
       </c>
@@ -3692,7 +3729,7 @@
         <v>25484336</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>67206</v>
       </c>
@@ -3706,7 +3743,7 @@
         <v>21444682</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>67572</v>
       </c>
@@ -3720,7 +3757,7 @@
         <v>17913600</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>67937</v>
       </c>
@@ -3734,7 +3771,7 @@
         <v>14847173</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>68302</v>
       </c>
@@ -3748,7 +3785,7 @@
         <v>12203344</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68667</v>
       </c>
@@ -3762,7 +3799,7 @@
         <v>9941649</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69033</v>
       </c>
@@ -3776,7 +3813,7 @@
         <v>8023034</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69398</v>
       </c>
@@ -3790,7 +3827,7 @@
         <v>6410121</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>69763</v>
       </c>
@@ -3804,7 +3841,7 @@
         <v>5067262</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>70128</v>
       </c>
@@ -3818,7 +3855,7 @@
         <v>3960593</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>70494</v>
       </c>
@@ -3832,7 +3869,7 @@
         <v>3058449</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>70859</v>
       </c>
@@ -3846,7 +3883,7 @@
         <v>2331583</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>71224</v>
       </c>
@@ -3860,7 +3897,7 @@
         <v>1753292</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>71589</v>
       </c>
@@ -3874,7 +3911,7 @@
         <v>1299479</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>71955</v>
       </c>
@@ -3888,7 +3925,7 @@
         <v>948586</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>72320</v>
       </c>
@@ -3902,7 +3939,7 @@
         <v>681542</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>72685</v>
       </c>
@@ -3916,7 +3953,7 @@
         <v>481719</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>73050</v>
       </c>
@@ -3939,17 +3976,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60852784-4F20-47CA-A3BD-A7CCB08511E9}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3963,11 +4001,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44196</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1126477546.4869819</v>
       </c>
       <c r="C2">
@@ -3977,7 +4015,7 @@
         <v>372907665</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44561</v>
       </c>
@@ -3991,7 +4029,7 @@
         <v>409584298</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -4005,7 +4043,7 @@
         <v>443363866</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45291</v>
       </c>
@@ -4019,7 +4057,7 @@
         <v>474322697</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45657</v>
       </c>
@@ -4033,7 +4071,7 @@
         <v>500844837</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>46022</v>
       </c>
@@ -4047,7 +4085,7 @@
         <v>522432352</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>46387</v>
       </c>
@@ -4061,7 +4099,7 @@
         <v>542860942</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>46752</v>
       </c>
@@ -4075,7 +4113,7 @@
         <v>560830549</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>47118</v>
       </c>
@@ -4089,7 +4127,7 @@
         <v>575397425</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>47483</v>
       </c>
@@ -4103,7 +4141,7 @@
         <v>586858685</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>47848</v>
       </c>
@@ -4117,7 +4155,7 @@
         <v>595893530</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>48213</v>
       </c>
@@ -4131,7 +4169,7 @@
         <v>603863653</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>48579</v>
       </c>
@@ -4145,7 +4183,7 @@
         <v>610486380</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>48944</v>
       </c>
@@ -4159,7 +4197,7 @@
         <v>615374537</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>49309</v>
       </c>
@@ -4173,7 +4211,7 @@
         <v>618327565</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>49674</v>
       </c>
@@ -4187,7 +4225,7 @@
         <v>619976237</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>50040</v>
       </c>
@@ -4201,7 +4239,7 @@
         <v>621940722</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>50405</v>
       </c>
@@ -4215,7 +4253,7 @@
         <v>624327762</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>50770</v>
       </c>
@@ -4229,7 +4267,7 @@
         <v>625934854</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>51135</v>
       </c>
@@ -4243,7 +4281,7 @@
         <v>626050704</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>51501</v>
       </c>
@@ -4257,7 +4295,7 @@
         <v>624525527</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>51866</v>
       </c>
@@ -4271,7 +4309,7 @@
         <v>621329593</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>52231</v>
       </c>
@@ -4285,7 +4323,7 @@
         <v>616450203</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>52596</v>
       </c>
@@ -4299,7 +4337,7 @@
         <v>610009688</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>52962</v>
       </c>
@@ -4313,7 +4351,7 @@
         <v>601859474</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>53327</v>
       </c>
@@ -4327,7 +4365,7 @@
         <v>591890495</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>53692</v>
       </c>
@@ -4341,7 +4379,7 @@
         <v>580248851</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>54057</v>
       </c>
@@ -4355,7 +4393,7 @@
         <v>566904504</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>54423</v>
       </c>
@@ -4369,7 +4407,7 @@
         <v>551973531</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>54788</v>
       </c>
@@ -4383,7 +4421,7 @@
         <v>535620610</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>55153</v>
       </c>
@@ -4397,7 +4435,7 @@
         <v>523623493</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>55518</v>
       </c>
@@ -4411,7 +4449,7 @@
         <v>593350470</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>55884</v>
       </c>
@@ -4425,7 +4463,7 @@
         <v>648381204</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>56249</v>
       </c>
@@ -4439,7 +4477,7 @@
         <v>612073537</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>56614</v>
       </c>
@@ -4453,7 +4491,7 @@
         <v>575351787</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>56979</v>
       </c>
@@ -4467,7 +4505,7 @@
         <v>538567562</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>57345</v>
       </c>
@@ -4481,7 +4519,7 @@
         <v>502119791</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>57710</v>
       </c>
@@ -4495,7 +4533,7 @@
         <v>466352387</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>58075</v>
       </c>
@@ -4509,7 +4547,7 @@
         <v>431552916</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>58440</v>
       </c>
@@ -4523,7 +4561,7 @@
         <v>397928242</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>58806</v>
       </c>
@@ -4537,7 +4575,7 @@
         <v>365665062</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>59171</v>
       </c>
@@ -4551,7 +4589,7 @@
         <v>334916307</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>59536</v>
       </c>
@@ -4565,7 +4603,7 @@
         <v>305783598</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>59901</v>
       </c>
@@ -4579,7 +4617,7 @@
         <v>278346158</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>60267</v>
       </c>
@@ -4593,7 +4631,7 @@
         <v>252644815</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>60632</v>
       </c>
@@ -4607,7 +4645,7 @@
         <v>228681342</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>60997</v>
       </c>
@@ -4621,7 +4659,7 @@
         <v>206426604</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>61362</v>
       </c>
@@ -4635,7 +4673,7 @@
         <v>185833396</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>61728</v>
       </c>
@@ -4649,7 +4687,7 @@
         <v>166842154</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>62093</v>
       </c>
@@ -4663,7 +4701,7 @@
         <v>149382467</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>62458</v>
       </c>
@@ -4677,7 +4715,7 @@
         <v>133376155</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>62823</v>
       </c>
@@ -4691,7 +4729,7 @@
         <v>118738271</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>63189</v>
       </c>
@@ -4705,7 +4743,7 @@
         <v>105381980</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>63554</v>
       </c>
@@ -4719,7 +4757,7 @@
         <v>93222296</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>63919</v>
       </c>
@@ -4733,7 +4771,7 @@
         <v>82177742</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>64284</v>
       </c>
@@ -4747,7 +4785,7 @@
         <v>72170614</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>64650</v>
       </c>
@@ -4761,7 +4799,7 @@
         <v>63127319</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>65015</v>
       </c>
@@ -4775,7 +4813,7 @@
         <v>54975531</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>65380</v>
       </c>
@@ -4789,7 +4827,7 @@
         <v>47654068</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>65745</v>
       </c>
@@ -4803,7 +4841,7 @@
         <v>41098526</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>66111</v>
       </c>
@@ -4817,7 +4855,7 @@
         <v>35250658</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>66476</v>
       </c>
@@ -4831,7 +4869,7 @@
         <v>30055953</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>66841</v>
       </c>
@@ -4845,7 +4883,7 @@
         <v>25463586</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>67206</v>
       </c>
@@ -4859,7 +4897,7 @@
         <v>21425380</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>67572</v>
       </c>
@@ -4873,7 +4911,7 @@
         <v>17895539</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>67937</v>
       </c>
@@ -4887,7 +4925,7 @@
         <v>14830190</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>68302</v>
       </c>
@@ -4901,7 +4939,7 @@
         <v>12187311</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68667</v>
       </c>
@@ -4915,7 +4953,7 @@
         <v>9926465</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69033</v>
       </c>
@@ -4929,7 +4967,7 @@
         <v>8008624</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69398</v>
       </c>
@@ -4943,7 +4981,7 @@
         <v>6396426</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>69763</v>
       </c>
@@ -4957,7 +4995,7 @@
         <v>5054242</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>70128</v>
       </c>
@@ -4971,7 +5009,7 @@
         <v>3948221</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>70494</v>
       </c>
@@ -4985,7 +5023,7 @@
         <v>3046709</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>70859</v>
       </c>
@@ -4999,7 +5037,7 @@
         <v>2320467</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>71224</v>
       </c>
@@ -5013,7 +5051,7 @@
         <v>1742794</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>71589</v>
       </c>
@@ -5027,7 +5065,7 @@
         <v>1289597</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>71955</v>
       </c>
@@ -5041,7 +5079,7 @@
         <v>939324</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>72320</v>
       </c>
@@ -5055,7 +5093,7 @@
         <v>672906</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>72685</v>
       </c>
@@ -5069,7 +5107,7 @@
         <v>473714</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>73050</v>
       </c>
@@ -5081,6 +5119,1158 @@
       </c>
       <c r="D81">
         <v>327470</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D42817-0D4E-41D7-A4D8-F6F8A83CA585}">
+  <dimension ref="A1:D81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B2">
+        <v>1213627245.4200001</v>
+      </c>
+      <c r="C2">
+        <v>262659142.11859041</v>
+      </c>
+      <c r="D2">
+        <v>424015774.05129546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B3">
+        <v>1269439337.4100001</v>
+      </c>
+      <c r="C3">
+        <v>293647149.88196254</v>
+      </c>
+      <c r="D3">
+        <v>457065275.86267245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45291</v>
+      </c>
+      <c r="B4">
+        <v>1329411806.5599999</v>
+      </c>
+      <c r="C4">
+        <v>325472217.7202239</v>
+      </c>
+      <c r="D4">
+        <v>488405515.40864128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45657</v>
+      </c>
+      <c r="B5">
+        <v>1388611025.73</v>
+      </c>
+      <c r="C5">
+        <v>357745042.83172649</v>
+      </c>
+      <c r="D5">
+        <v>516863212.12272674</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B6">
+        <v>1447252732.9300001</v>
+      </c>
+      <c r="C6">
+        <v>390014113.85726863</v>
+      </c>
+      <c r="D6">
+        <v>540963075.93295217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B7">
+        <v>1502556821.4100001</v>
+      </c>
+      <c r="C7">
+        <v>422013825.0374046</v>
+      </c>
+      <c r="D7">
+        <v>563238770.2817446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B8">
+        <v>1552050232.1099999</v>
+      </c>
+      <c r="C8">
+        <v>453322828.62352318</v>
+      </c>
+      <c r="D8">
+        <v>583346925.73878193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>47118</v>
+      </c>
+      <c r="B9">
+        <v>1593034537.02</v>
+      </c>
+      <c r="C9">
+        <v>483346116.48300433</v>
+      </c>
+      <c r="D9">
+        <v>600262968.05763745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>47483</v>
+      </c>
+      <c r="B10">
+        <v>1628726662.4400001</v>
+      </c>
+      <c r="C10">
+        <v>512106964.06418198</v>
+      </c>
+      <c r="D10">
+        <v>614431256.93380749</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>47848</v>
+      </c>
+      <c r="B11">
+        <v>1660081684.1800001</v>
+      </c>
+      <c r="C11">
+        <v>539789358.94055665</v>
+      </c>
+      <c r="D11">
+        <v>626399997.06846392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>48213</v>
+      </c>
+      <c r="B12">
+        <v>1685320815.6700001</v>
+      </c>
+      <c r="C12">
+        <v>565726574.31639421</v>
+      </c>
+      <c r="D12">
+        <v>637224083.46310794</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>48579</v>
+      </c>
+      <c r="B13">
+        <v>1703990977.27</v>
+      </c>
+      <c r="C13">
+        <v>589160498.98871207</v>
+      </c>
+      <c r="D13">
+        <v>646549908.19188178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>48944</v>
+      </c>
+      <c r="B14">
+        <v>1715411808.22</v>
+      </c>
+      <c r="C14">
+        <v>609690875.99307108</v>
+      </c>
+      <c r="D14">
+        <v>654004643.88014925</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>49309</v>
+      </c>
+      <c r="B15">
+        <v>1717248496.4400001</v>
+      </c>
+      <c r="C15">
+        <v>627819121.28365505</v>
+      </c>
+      <c r="D15">
+        <v>659341735.95668685</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>49674</v>
+      </c>
+      <c r="B16">
+        <v>1714174177.53</v>
+      </c>
+      <c r="C16">
+        <v>643839652.0939014</v>
+      </c>
+      <c r="D16">
+        <v>663292666.11693799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>50040</v>
+      </c>
+      <c r="B17">
+        <v>1703777499.29</v>
+      </c>
+      <c r="C17">
+        <v>657553816.45534825</v>
+      </c>
+      <c r="D17">
+        <v>667565374.02980375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>50405</v>
+      </c>
+      <c r="B18">
+        <v>1687725805.77</v>
+      </c>
+      <c r="C18">
+        <v>668853099.22501326</v>
+      </c>
+      <c r="D18">
+        <v>672200031.14548743</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>50770</v>
+      </c>
+      <c r="B19">
+        <v>1666142611.4100001</v>
+      </c>
+      <c r="C19">
+        <v>678179158.23396182</v>
+      </c>
+      <c r="D19">
+        <v>675957099.92138398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>51135</v>
+      </c>
+      <c r="B20">
+        <v>1640558569.6800001</v>
+      </c>
+      <c r="C20">
+        <v>685713582.29591227</v>
+      </c>
+      <c r="D20">
+        <v>678178758.23305225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>51501</v>
+      </c>
+      <c r="B21">
+        <v>1608435694.3599999</v>
+      </c>
+      <c r="C21">
+        <v>691498472.09422243</v>
+      </c>
+      <c r="D21">
+        <v>678671493.26447356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>51866</v>
+      </c>
+      <c r="B22">
+        <v>1573397888.3099999</v>
+      </c>
+      <c r="C22">
+        <v>695759069.0108918</v>
+      </c>
+      <c r="D22">
+        <v>677334354.24249148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>52231</v>
+      </c>
+      <c r="B23">
+        <v>1534121579.9400001</v>
+      </c>
+      <c r="C23">
+        <v>698467634.44513285</v>
+      </c>
+      <c r="D23">
+        <v>674115982.06267798</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>52596</v>
+      </c>
+      <c r="B24">
+        <v>1492897667.3299999</v>
+      </c>
+      <c r="C24">
+        <v>699372552.20554912</v>
+      </c>
+      <c r="D24">
+        <v>669200470.54096711</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>52962</v>
+      </c>
+      <c r="B25">
+        <v>1446057869.3800001</v>
+      </c>
+      <c r="C25">
+        <v>697911404.50421655</v>
+      </c>
+      <c r="D25">
+        <v>662461057.13785613</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>53327</v>
+      </c>
+      <c r="B26">
+        <v>1394912230.05</v>
+      </c>
+      <c r="C26">
+        <v>693950320.83901548</v>
+      </c>
+      <c r="D26">
+        <v>653748623.38036883</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>53692</v>
+      </c>
+      <c r="B27">
+        <v>1341111105.48</v>
+      </c>
+      <c r="C27">
+        <v>688190164.6527648</v>
+      </c>
+      <c r="D27">
+        <v>643184810.84966457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>54057</v>
+      </c>
+      <c r="B28">
+        <v>1283077822.3499999</v>
+      </c>
+      <c r="C28">
+        <v>680810227.93361127</v>
+      </c>
+      <c r="D28">
+        <v>630714294.71687984</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>54423</v>
+      </c>
+      <c r="B29">
+        <v>1221426484.76</v>
+      </c>
+      <c r="C29">
+        <v>671477097.23769784</v>
+      </c>
+      <c r="D29">
+        <v>616448234.49187398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>54788</v>
+      </c>
+      <c r="B30">
+        <v>1156480555.03</v>
+      </c>
+      <c r="C30">
+        <v>659790275.68906605</v>
+      </c>
+      <c r="D30">
+        <v>600573880.64061856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>55153</v>
+      </c>
+      <c r="B31">
+        <v>1087328191.0699999</v>
+      </c>
+      <c r="C31">
+        <v>645402297.92353272</v>
+      </c>
+      <c r="D31">
+        <v>588969020.39382529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>55518</v>
+      </c>
+      <c r="B32">
+        <v>1018731306.6</v>
+      </c>
+      <c r="C32">
+        <v>628845197.47830248</v>
+      </c>
+      <c r="D32">
+        <v>654617847.92331505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>55884</v>
+      </c>
+      <c r="B33">
+        <v>946062645.11000001</v>
+      </c>
+      <c r="C33">
+        <v>610738672.94004881</v>
+      </c>
+      <c r="D33">
+        <v>700458249.75067556</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>56249</v>
+      </c>
+      <c r="B34">
+        <v>874426793.99000001</v>
+      </c>
+      <c r="C34">
+        <v>591468532.89777243</v>
+      </c>
+      <c r="D34">
+        <v>661931725.8571496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>56614</v>
+      </c>
+      <c r="B35">
+        <v>804894914.36000001</v>
+      </c>
+      <c r="C35">
+        <v>571328378.64560461</v>
+      </c>
+      <c r="D35">
+        <v>622775801.94075274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>56979</v>
+      </c>
+      <c r="B36">
+        <v>736476970.73000002</v>
+      </c>
+      <c r="C36">
+        <v>550575773.560853</v>
+      </c>
+      <c r="D36">
+        <v>583337433.7355845</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>57345</v>
+      </c>
+      <c r="B37">
+        <v>670670606.39999998</v>
+      </c>
+      <c r="C37">
+        <v>529361071.24776328</v>
+      </c>
+      <c r="D37">
+        <v>550942897.15521514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>57710</v>
+      </c>
+      <c r="B38">
+        <v>608971991.13</v>
+      </c>
+      <c r="C38">
+        <v>507995421.29784733</v>
+      </c>
+      <c r="D38">
+        <v>520626161.2241593</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>58075</v>
+      </c>
+      <c r="B39">
+        <v>551270901.30999994</v>
+      </c>
+      <c r="C39">
+        <v>486650182.30266255</v>
+      </c>
+      <c r="D39">
+        <v>484646188.42140341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>58440</v>
+      </c>
+      <c r="B40">
+        <v>496897872.72000003</v>
+      </c>
+      <c r="C40">
+        <v>465188469.71478313</v>
+      </c>
+      <c r="D40">
+        <v>449628286.54489565</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>58806</v>
+      </c>
+      <c r="B41">
+        <v>446392131.32999998</v>
+      </c>
+      <c r="C41">
+        <v>443033598.73878902</v>
+      </c>
+      <c r="D41">
+        <v>415783852.15479821</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>59171</v>
+      </c>
+      <c r="B42">
+        <v>399563847.73000002</v>
+      </c>
+      <c r="C42">
+        <v>420445956.41725731</v>
+      </c>
+      <c r="D42">
+        <v>383281984.03516048</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>59536</v>
+      </c>
+      <c r="B43">
+        <v>356279034.27999997</v>
+      </c>
+      <c r="C43">
+        <v>398395271.62121898</v>
+      </c>
+      <c r="D43">
+        <v>352252008.24275076</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>59901</v>
+      </c>
+      <c r="B44">
+        <v>316424106.57999998</v>
+      </c>
+      <c r="C44">
+        <v>377046021.55714232</v>
+      </c>
+      <c r="D44">
+        <v>322811822.83203197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>60267</v>
+      </c>
+      <c r="B45">
+        <v>279903321.61000001</v>
+      </c>
+      <c r="C45">
+        <v>355000804.03109366</v>
+      </c>
+      <c r="D45">
+        <v>295036481.24885195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>60632</v>
+      </c>
+      <c r="B46">
+        <v>246586556.37</v>
+      </c>
+      <c r="C46">
+        <v>332154553.53467178</v>
+      </c>
+      <c r="D46">
+        <v>268953117.07541275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>60997</v>
+      </c>
+      <c r="B47">
+        <v>216326458.81999999</v>
+      </c>
+      <c r="C47">
+        <v>309922789.65834373</v>
+      </c>
+      <c r="D47">
+        <v>244555347.35137379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>61362</v>
+      </c>
+      <c r="B48">
+        <v>188953210.80000001</v>
+      </c>
+      <c r="C48">
+        <v>288462425.10470229</v>
+      </c>
+      <c r="D48">
+        <v>221813807.83115515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>61728</v>
+      </c>
+      <c r="B49">
+        <v>164278363.03999999</v>
+      </c>
+      <c r="C49">
+        <v>267788518.32217118</v>
+      </c>
+      <c r="D49">
+        <v>200684753.11110151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>62093</v>
+      </c>
+      <c r="B50">
+        <v>142120875.03999999</v>
+      </c>
+      <c r="C50">
+        <v>247910874.3647587</v>
+      </c>
+      <c r="D50">
+        <v>181108394.59670976</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>62458</v>
+      </c>
+      <c r="B51">
+        <v>122300164.87</v>
+      </c>
+      <c r="C51">
+        <v>228839536.62758189</v>
+      </c>
+      <c r="D51">
+        <v>163019465.61501855</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>62823</v>
+      </c>
+      <c r="B52">
+        <v>104640857.15000001</v>
+      </c>
+      <c r="C52">
+        <v>210580402.0469687</v>
+      </c>
+      <c r="D52">
+        <v>146345463.57891101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>63189</v>
+      </c>
+      <c r="B53">
+        <v>88974717.420000002</v>
+      </c>
+      <c r="C53">
+        <v>193136441.03002697</v>
+      </c>
+      <c r="D53">
+        <v>131006499.70167373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>63554</v>
+      </c>
+      <c r="B54">
+        <v>75143356.760000005</v>
+      </c>
+      <c r="C54">
+        <v>176511591.38236633</v>
+      </c>
+      <c r="D54">
+        <v>116922505.81858487</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>63919</v>
+      </c>
+      <c r="B55">
+        <v>62997487.109999999</v>
+      </c>
+      <c r="C55">
+        <v>160710529.94410756</v>
+      </c>
+      <c r="D55">
+        <v>104016625.59105338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>64284</v>
+      </c>
+      <c r="B56">
+        <v>52396035.57</v>
+      </c>
+      <c r="C56">
+        <v>145737855.10951975</v>
+      </c>
+      <c r="D56">
+        <v>92214859.748915792</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>64650</v>
+      </c>
+      <c r="B57">
+        <v>43205358.789999999</v>
+      </c>
+      <c r="C57">
+        <v>131597372.44534118</v>
+      </c>
+      <c r="D57">
+        <v>81446613.403591797</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>65015</v>
+      </c>
+      <c r="B58">
+        <v>35298638.060000002</v>
+      </c>
+      <c r="C58">
+        <v>118291129.90186666</v>
+      </c>
+      <c r="D58">
+        <v>71642420.750188708</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>65380</v>
+      </c>
+      <c r="B59">
+        <v>28554178.98</v>
+      </c>
+      <c r="C59">
+        <v>105819098.00988619</v>
+      </c>
+      <c r="D59">
+        <v>62743807.462651148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>65745</v>
+      </c>
+      <c r="B60">
+        <v>22855775.390000001</v>
+      </c>
+      <c r="C60">
+        <v>94179444.085991025</v>
+      </c>
+      <c r="D60">
+        <v>54688813.412922546</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>66111</v>
+      </c>
+      <c r="B61">
+        <v>18092107.66</v>
+      </c>
+      <c r="C61">
+        <v>83367610.267755643</v>
+      </c>
+      <c r="D61">
+        <v>47421568.635305598</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>66476</v>
+      </c>
+      <c r="B62">
+        <v>14154394.720000001</v>
+      </c>
+      <c r="C62">
+        <v>73375064.046192244</v>
+      </c>
+      <c r="D62">
+        <v>40889651.017982721</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>66841</v>
+      </c>
+      <c r="B63">
+        <v>10939135.16</v>
+      </c>
+      <c r="C63">
+        <v>64188864.743345246</v>
+      </c>
+      <c r="D63">
+        <v>35044137.800875515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>67206</v>
+      </c>
+      <c r="B64">
+        <v>8349468.79</v>
+      </c>
+      <c r="C64">
+        <v>55791231.950221665</v>
+      </c>
+      <c r="D64">
+        <v>29838429.274073739</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>67572</v>
+      </c>
+      <c r="B65">
+        <v>6292149.3200000003</v>
+      </c>
+      <c r="C65">
+        <v>48159858.818404883</v>
+      </c>
+      <c r="D65">
+        <v>25227871.031134009</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>67937</v>
+      </c>
+      <c r="B66">
+        <v>4681602.5999999996</v>
+      </c>
+      <c r="C66">
+        <v>41268534.154762141</v>
+      </c>
+      <c r="D66">
+        <v>21169250.973493949</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>68302</v>
+      </c>
+      <c r="B67">
+        <v>3442042.69</v>
+      </c>
+      <c r="C67">
+        <v>35088009.083248474</v>
+      </c>
+      <c r="D67">
+        <v>17620572.402046002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>68667</v>
+      </c>
+      <c r="B68">
+        <v>2501370.7400000002</v>
+      </c>
+      <c r="C68">
+        <v>29585938.246604353</v>
+      </c>
+      <c r="D68">
+        <v>14540723.948767908</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>69033</v>
+      </c>
+      <c r="B69">
+        <v>1801365.37</v>
+      </c>
+      <c r="C69">
+        <v>24727341.601288818</v>
+      </c>
+      <c r="D69">
+        <v>11889269.356152872</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>69398</v>
+      </c>
+      <c r="B70">
+        <v>1288860.3899999999</v>
+      </c>
+      <c r="C70">
+        <v>20474491.845707566</v>
+      </c>
+      <c r="D70">
+        <v>9626534.1361398604</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>69763</v>
+      </c>
+      <c r="B71">
+        <v>921855.78</v>
+      </c>
+      <c r="C71">
+        <v>16786740.768610012</v>
+      </c>
+      <c r="D71">
+        <v>7713663.9164395034</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>70128</v>
+      </c>
+      <c r="B72">
+        <v>662042.9</v>
+      </c>
+      <c r="C72">
+        <v>13620604.391801871</v>
+      </c>
+      <c r="D72">
+        <v>6112659.9901514407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>70494</v>
+      </c>
+      <c r="B73">
+        <v>482102.5</v>
+      </c>
+      <c r="C73">
+        <v>10930497.129484463</v>
+      </c>
+      <c r="D73">
+        <v>4786871.5371281961</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>70859</v>
+      </c>
+      <c r="B74">
+        <v>358689.48</v>
+      </c>
+      <c r="C74">
+        <v>8669542.5472833775</v>
+      </c>
+      <c r="D74">
+        <v>3701449.3464187072</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>71224</v>
+      </c>
+      <c r="B75">
+        <v>274637.03000000003</v>
+      </c>
+      <c r="C75">
+        <v>6790276.0898670088</v>
+      </c>
+      <c r="D75">
+        <v>2823622.4151561731</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>71589</v>
+      </c>
+      <c r="B76">
+        <v>217960.23</v>
+      </c>
+      <c r="C76">
+        <v>5246397.4382971078</v>
+      </c>
+      <c r="D76">
+        <v>2123037.990304952</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>71955</v>
+      </c>
+      <c r="B77">
+        <v>179288.09</v>
+      </c>
+      <c r="C77">
+        <v>3994524.3894720506</v>
+      </c>
+      <c r="D77">
+        <v>1571921.1952047334</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>72320</v>
+      </c>
+      <c r="B78">
+        <v>152044.59</v>
+      </c>
+      <c r="C78">
+        <v>2993947.7880517975</v>
+      </c>
+      <c r="D78">
+        <v>1145057.9585733623</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>72685</v>
+      </c>
+      <c r="B79">
+        <v>131376.57</v>
+      </c>
+      <c r="C79">
+        <v>2206544.1572660301</v>
+      </c>
+      <c r="D79">
+        <v>819894.01799540711</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>73050</v>
+      </c>
+      <c r="B80">
+        <v>116384.47</v>
+      </c>
+      <c r="C80">
+        <v>1597268.9566045678</v>
+      </c>
+      <c r="D80">
+        <v>576571.23908656347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>73415</v>
+      </c>
+      <c r="B81">
+        <v>104942.29</v>
+      </c>
+      <c r="C81">
+        <v>1134320.121852173</v>
+      </c>
+      <c r="D81">
+        <v>397899.28710025933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>